<commit_message>
More reorganization, some updates to python 3
</commit_message>
<xml_diff>
--- a/syllabus-2016.xlsx
+++ b/syllabus-2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19280" yWindow="2100" windowWidth="31900" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="3400" yWindow="2500" windowWidth="31900" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="134">
   <si>
     <t>Week</t>
   </si>
@@ -278,12 +278,6 @@
     <t>Intro and Setup</t>
   </si>
   <si>
-    <t>02 - Strings-lists-dictionaries.ipynb</t>
-  </si>
-  <si>
-    <t>01 - Introduction-to-jupyter-notebooks-and-python.ipynb</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -293,24 +287,12 @@
     <t>Notebook / Presentation</t>
   </si>
   <si>
-    <t>03 - Planning-code-prime-numbers-example.ipynb</t>
-  </si>
-  <si>
     <t>Session</t>
   </si>
   <si>
-    <t>Web Mapping with Leaflet (Sam Maurer)</t>
-  </si>
-  <si>
-    <t>Solving Problems with Code, and Wordpress tutorial</t>
-  </si>
-  <si>
     <t>Data Cleaning, QGIS Tutorial</t>
   </si>
   <si>
-    <t>[PW] assign exercise 6: Extract data via API</t>
-  </si>
-  <si>
     <t>[PW] assign exercise 4: python script</t>
   </si>
   <si>
@@ -326,15 +308,9 @@
     <t>[PW/GB] Install Anaconda, Create a Jupyter Notebook, Setup OCF, assign exercise 1: Initial Jupyter Notebook and OCF setup</t>
   </si>
   <si>
-    <t>[PW] assign exercise 8: web mapping blog post</t>
-  </si>
-  <si>
     <t>[PW] assign exercise 9: data science insights</t>
   </si>
   <si>
-    <t>Geocoding</t>
-  </si>
-  <si>
     <t>[PW] assign exercise 3: python script</t>
   </si>
   <si>
@@ -411,6 +387,48 @@
   </si>
   <si>
     <t>Web Mapping with ViziCities</t>
+  </si>
+  <si>
+    <t>Wordpress tutorial</t>
+  </si>
+  <si>
+    <t>Introduction-to-jupyter-notebooks-and-python.ipynb</t>
+  </si>
+  <si>
+    <t>Strings-lists-dictionaries.ipynb</t>
+  </si>
+  <si>
+    <t>Planning-code-prime-numbers-example.ipynb</t>
+  </si>
+  <si>
+    <t>string-methods-conditions-iteration.ipynb</t>
+  </si>
+  <si>
+    <t>String Methods, Conditions, Booleans and Iteration</t>
+  </si>
+  <si>
+    <t>From  Lists, Data Cleaning</t>
+  </si>
+  <si>
+    <t>Geocoding and Reverse Geocoding</t>
+  </si>
+  <si>
+    <t>[SM] assign exercise 6: Extract data via API</t>
+  </si>
+  <si>
+    <t>Web Programming with Javascript</t>
+  </si>
+  <si>
+    <t>Web Mapping with Leaflet</t>
+  </si>
+  <si>
+    <t>[GB] assign exercise 8: web mapping blog post</t>
+  </si>
+  <si>
+    <t>[PW] ET Confirmed</t>
+  </si>
+  <si>
+    <t>[PW/SB]</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1077,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1078,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1090,18 +1108,18 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1124,16 +1142,16 @@
         <v>82</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1153,13 +1171,13 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1173,16 +1191,16 @@
         <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1200,7 +1218,7 @@
         <v>35</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1217,16 +1235,16 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" t="s">
-        <v>88</v>
+        <v>105</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1240,13 +1258,16 @@
         <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>125</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1260,13 +1281,16 @@
         <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1280,13 +1304,16 @@
         <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="G10" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1300,18 +1327,18 @@
         <v>54</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1328,13 +1355,13 @@
         <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1348,13 +1375,13 @@
         <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1368,13 +1395,13 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1388,13 +1415,13 @@
         <v>58</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1408,13 +1435,13 @@
         <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1428,13 +1455,13 @@
         <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1448,13 +1475,13 @@
         <v>61</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1468,13 +1495,13 @@
         <v>62</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1488,18 +1515,18 @@
         <v>63</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1518,13 +1545,13 @@
         <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1538,13 +1565,13 @@
         <v>65</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1557,14 +1584,14 @@
       <c r="C25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>104</v>
+      <c r="D25" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>80</v>
@@ -1580,14 +1607,14 @@
       <c r="C26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>101</v>
+      <c r="D26" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1600,14 +1627,14 @@
       <c r="C27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>22</v>
+      <c r="D27" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1621,13 +1648,13 @@
         <v>69</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1641,13 +1668,13 @@
         <v>70</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1661,13 +1688,13 @@
         <v>71</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1743,9 +1770,6 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D36"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D37"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">

</xml_diff>

<commit_message>
Updated syllabus, minor updates to Session 21
</commit_message>
<xml_diff>
--- a/syllabus-2016.xlsx
+++ b/syllabus-2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="2500" windowWidth="31900" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="19220" yWindow="460" windowWidth="31900" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="133">
   <si>
     <t>Week</t>
   </si>
@@ -296,9 +296,6 @@
     <t>[PW] assign exercise 4: python script</t>
   </si>
   <si>
-    <t>Working with APIs (Sam Maurer)</t>
-  </si>
-  <si>
     <t>Part 1:  Introduction to Programming, Data Acquisition, and Basic Geospatial Data Visualization</t>
   </si>
   <si>
@@ -314,9 +311,6 @@
     <t>[PW] assign exercise 3: python script</t>
   </si>
   <si>
-    <t>[PW] assign exercise 7: matplotlib/pandas visualization</t>
-  </si>
-  <si>
     <t>Statistical Analysis with Statsmodels</t>
   </si>
   <si>
@@ -356,9 +350,6 @@
     <t>Updated Status</t>
   </si>
   <si>
-    <t>[PW/GB]</t>
-  </si>
-  <si>
     <t>[GB]  assign exercise 2: create blog post with CartoDB viz</t>
   </si>
   <si>
@@ -377,9 +368,6 @@
     <t>Data Wrangling With Pandas</t>
   </si>
   <si>
-    <t>Data Visualization With Pandas</t>
-  </si>
-  <si>
     <t>Data Science With Pandas Part 1</t>
   </si>
   <si>
@@ -413,12 +401,6 @@
     <t>Geocoding and Reverse Geocoding</t>
   </si>
   <si>
-    <t>[SM] assign exercise 6: Extract data via API</t>
-  </si>
-  <si>
-    <t>Web Programming with Javascript</t>
-  </si>
-  <si>
     <t>Web Mapping with Leaflet</t>
   </si>
   <si>
@@ -429,6 +411,21 @@
   </si>
   <si>
     <t>[PW/SB]</t>
+  </si>
+  <si>
+    <t>Web Programming With Javascript</t>
+  </si>
+  <si>
+    <t>[PW] assign exercise 6: matplotlib/pandas visualization</t>
+  </si>
+  <si>
+    <t>[SM] assign exercise 7: Extract data via API</t>
+  </si>
+  <si>
+    <t>Data Visualization With Pandas, Matplotlib, and Plotly</t>
+  </si>
+  <si>
+    <t>Working with APIs in Python (Sam Maurer)</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1074,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1108,18 +1105,18 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1142,16 +1139,16 @@
         <v>82</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1171,13 +1168,13 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1191,13 +1188,13 @@
         <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>83</v>
@@ -1235,16 +1232,16 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>83</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1258,16 +1255,16 @@
         <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1281,13 +1278,13 @@
         <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>84</v>
@@ -1304,16 +1301,16 @@
         <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1333,12 +1330,12 @@
         <v>11</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1355,13 +1352,13 @@
         <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1375,13 +1372,13 @@
         <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1395,13 +1392,13 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1414,14 +1411,14 @@
       <c r="C16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>129</v>
+      <c r="D16" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1435,13 +1432,13 @@
         <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1454,14 +1451,14 @@
       <c r="C18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>115</v>
+      <c r="D18" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1475,13 +1472,13 @@
         <v>61</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1495,13 +1492,13 @@
         <v>62</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1515,18 +1512,18 @@
         <v>63</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1545,13 +1542,13 @@
         <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1565,13 +1562,13 @@
         <v>65</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1585,13 +1582,13 @@
         <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>80</v>
@@ -1608,13 +1605,13 @@
         <v>67</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1628,13 +1625,13 @@
         <v>68</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1648,13 +1645,13 @@
         <v>69</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1668,13 +1665,13 @@
         <v>70</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1688,13 +1685,13 @@
         <v>71</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Confirmed guest presentations, draft final schedule
</commit_message>
<xml_diff>
--- a/syllabus-2016.xlsx
+++ b/syllabus-2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="3540" windowWidth="29540" windowHeight="22180" tabRatio="500"/>
+    <workbookView xWindow="740" yWindow="580" windowWidth="29540" windowHeight="22180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -348,9 +348,6 @@
     <t>Pandas Basics Part 2</t>
   </si>
   <si>
-    <t>Github and Version Control</t>
-  </si>
-  <si>
     <t>Data Wrangling With Pandas</t>
   </si>
   <si>
@@ -421,6 +418,9 @@
   </si>
   <si>
     <t>Part 3:  More Advanced Topics in Spatial Analysis and Web Geospatial Data Visualization</t>
+  </si>
+  <si>
+    <t>Scenario Planning With UrbanFootprint (Joe Distefano)</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -591,6 +591,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -631,7 +645,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -692,6 +706,13 @@
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -736,6 +757,13 @@
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1073,7 +1101,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:D30"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1144,7 +1172,7 @@
         <v>101</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>99</v>
@@ -1170,7 +1198,7 @@
         <v>101</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>99</v>
@@ -1187,7 +1215,7 @@
         <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>7</v>
@@ -1231,7 +1259,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>102</v>
@@ -1254,7 +1282,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>93</v>
@@ -1263,7 +1291,7 @@
         <v>102</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1280,7 +1308,7 @@
         <v>100</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>102</v>
@@ -1300,7 +1328,7 @@
         <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>88</v>
@@ -1309,7 +1337,7 @@
         <v>102</v>
       </c>
       <c r="G10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1391,10 +1419,10 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>102</v>
@@ -1411,7 +1439,7 @@
         <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>11</v>
@@ -1431,10 +1459,10 @@
         <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>102</v>
@@ -1451,7 +1479,7 @@
         <v>60</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>7</v>
@@ -1471,10 +1499,10 @@
         <v>61</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>102</v>
@@ -1491,7 +1519,7 @@
         <v>62</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>11</v>
@@ -1511,7 +1539,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>92</v>
@@ -1522,7 +1550,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1541,7 +1569,7 @@
         <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>11</v>
@@ -1624,7 +1652,7 @@
         <v>68</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>11</v>
@@ -1644,10 +1672,10 @@
         <v>69</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>102</v>
@@ -1664,7 +1692,7 @@
         <v>70</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Inserted session on OSM processing
</commit_message>
<xml_diff>
--- a/syllabus-2016.xlsx
+++ b/syllabus-2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="580" windowWidth="29540" windowHeight="22180" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="40" windowWidth="29540" windowHeight="22180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,6 @@
     <t>[PW] assign exercise 3: python script</t>
   </si>
   <si>
-    <t>Statistical Analysis with Statsmodels</t>
-  </si>
-  <si>
     <t>[PW] assign exercise 10: analysis of spatial data set</t>
   </si>
   <si>
@@ -421,6 +418,9 @@
   </si>
   <si>
     <t>Scenario Planning With UrbanFootprint (Joe Distefano)</t>
+  </si>
+  <si>
+    <t>Working with Open Street Map Data (Geoff)</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1101,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1132,13 +1132,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1">
@@ -1169,13 +1169,13 @@
         <v>91</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1195,13 +1195,13 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1215,13 +1215,13 @@
         <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>83</v>
@@ -1259,16 +1259,16 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>83</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1282,16 +1282,16 @@
         <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1305,13 +1305,13 @@
         <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>84</v>
@@ -1328,16 +1328,16 @@
         <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1357,7 +1357,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1379,13 +1379,13 @@
         <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1399,13 +1399,13 @@
         <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1419,13 +1419,13 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1439,13 +1439,13 @@
         <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1459,13 +1459,13 @@
         <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1479,13 +1479,13 @@
         <v>60</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1499,13 +1499,13 @@
         <v>61</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="F19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1519,13 +1519,13 @@
         <v>62</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1539,18 +1539,18 @@
         <v>63</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1569,13 +1569,13 @@
         <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1589,13 +1589,13 @@
         <v>65</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1609,13 +1609,13 @@
         <v>66</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>80</v>
@@ -1632,13 +1632,13 @@
         <v>67</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1652,13 +1652,13 @@
         <v>68</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1672,13 +1672,13 @@
         <v>69</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1692,13 +1692,13 @@
         <v>70</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1712,13 +1712,13 @@
         <v>71</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:7">

</xml_diff>

<commit_message>
Tweaks to the schedule
</commit_message>
<xml_diff>
--- a/syllabus-2016.xlsx
+++ b/syllabus-2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16820" yWindow="1760" windowWidth="29540" windowHeight="22180" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="3740" windowWidth="29540" windowHeight="22180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="139">
   <si>
     <t>Week</t>
   </si>
@@ -363,9 +363,6 @@
     <t>Web Mapping with Leaflet</t>
   </si>
   <si>
-    <t>Web Programming With Javascript</t>
-  </si>
-  <si>
     <t>Data Visualization With Pandas, Matplotlib, and Plotly</t>
   </si>
   <si>
@@ -403,9 +400,6 @@
   </si>
   <si>
     <t>Sam</t>
-  </si>
-  <si>
-    <t>Sam (or Geoff?)</t>
   </si>
   <si>
     <t>Sam B</t>
@@ -1125,7 +1119,7 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1154,7 +1148,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1195,10 +1189,10 @@
         <v>82</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>95</v>
@@ -1224,7 +1218,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3" t="s">
@@ -1251,7 +1245,7 @@
         <v>105</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3" t="s">
@@ -1294,10 +1288,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>96</v>
@@ -1323,10 +1317,10 @@
         <v>110</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>96</v>
@@ -1349,7 +1343,7 @@
         <v>94</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3" t="s">
@@ -1370,13 +1364,13 @@
         <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>96</v>
@@ -1399,7 +1393,7 @@
         <v>87</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="3" t="s">
@@ -1428,10 +1422,10 @@
         <v>99</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>96</v>
@@ -1451,7 +1445,7 @@
         <v>100</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="3" t="s">
@@ -1469,13 +1463,13 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>96</v>
@@ -1495,7 +1489,7 @@
         <v>101</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
@@ -1513,13 +1507,13 @@
         <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>96</v>
@@ -1536,10 +1530,10 @@
         <v>60</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="3" t="s">
@@ -1560,10 +1554,10 @@
         <v>112</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>96</v>
@@ -1583,7 +1577,7 @@
         <v>102</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="3" t="s">
@@ -1604,10 +1598,10 @@
         <v>103</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>96</v>
@@ -1615,7 +1609,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1638,7 +1632,7 @@
         <v>111</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="3" t="s">
@@ -1659,10 +1653,10 @@
         <v>98</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>96</v>
@@ -1679,10 +1673,10 @@
         <v>66</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
@@ -1706,7 +1700,7 @@
         <v>90</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="3" t="s">
@@ -1724,10 +1718,10 @@
         <v>68</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="3" t="s">
@@ -1745,10 +1739,10 @@
         <v>69</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
@@ -1769,7 +1763,7 @@
         <v>104</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="3" t="s">
@@ -1790,7 +1784,7 @@
         <v>91</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="3" t="s">

</xml_diff>

<commit_message>
Moved API session back to Oct 3
</commit_message>
<xml_diff>
--- a/syllabus-2016.xlsx
+++ b/syllabus-2016.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="42400" windowHeight="22200"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="139">
   <si>
     <t>Week</t>
   </si>
@@ -175,9 +183,6 @@
     <t>Data Visualization With Pandas, Matplotlib, and Plotly</t>
   </si>
   <si>
-    <t>assign exercise 6: matplotlib/pandas visualization</t>
-  </si>
-  <si>
     <t>Wed 5 Oct</t>
   </si>
   <si>
@@ -193,9 +198,6 @@
     <t>Sam</t>
   </si>
   <si>
-    <t>assign exercise 7: Extract data via API</t>
-  </si>
-  <si>
     <t>Wed 12 Oct</t>
   </si>
   <si>
@@ -428,33 +430,26 @@
   </si>
   <si>
     <t>Mon 14 Dec</t>
+  </si>
+  <si>
+    <t>assign exercise 6: Extract data via API</t>
+  </si>
+  <si>
+    <t>assign exercise 7: matplotlib/pandas visualization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -465,7 +460,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -510,76 +505,109 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="001FB714"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -705,7 +733,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -714,7 +742,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -723,7 +751,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -797,7 +825,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -805,7 +833,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -824,7 +852,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -854,7 +882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -880,7 +908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -906,7 +934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -932,7 +960,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -958,7 +986,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -984,7 +1012,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1010,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1036,7 +1064,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1062,7 +1090,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1075,9 +1103,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1092,7 +1126,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -1100,7 +1134,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1119,7 +1153,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1145,7 +1179,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1171,7 +1205,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1197,7 +1231,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1223,7 +1257,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1249,7 +1283,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1275,7 +1309,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1301,7 +1335,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1327,7 +1361,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1353,7 +1387,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1366,9 +1400,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1382,7 +1422,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1401,7 +1441,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1431,7 +1471,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1457,7 +1497,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1483,7 +1523,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1509,7 +1549,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1535,7 +1575,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1561,7 +1601,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1587,7 +1627,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1613,7 +1653,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1639,7 +1679,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1652,67 +1692,75 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV74"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5714" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.57812" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.86719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5781" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5781" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7344" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.1562" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5781" style="1" customWidth="1"/>
-    <col min="8" max="8" width="46.1562" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5781" style="1" customWidth="1"/>
-    <col min="10" max="256" width="10.5781" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="46.1640625" style="1" customWidth="1"/>
+    <col min="9" max="256" width="10.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="30" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:9" ht="17" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3"/>
@@ -1724,241 +1772,241 @@
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" ht="30" customHeight="1">
+    <row r="3" spans="1:9" ht="30" customHeight="1">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s" s="6">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s" s="6">
+      <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s" s="6">
+      <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s" s="6">
+      <c r="I3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="C4" t="s" s="6">
+      <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s" s="6">
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s" s="6">
+      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" t="s" s="6">
+      <c r="G4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s" s="6">
+      <c r="H4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s" s="6">
+      <c r="I4" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:9" ht="17" customHeight="1">
       <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="C5" t="s" s="6">
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s" s="6">
+      <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s" s="6">
+      <c r="E5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" t="s" s="6">
+      <c r="G5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H5" t="s" s="6">
+      <c r="H5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:9" ht="17" customHeight="1">
       <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" t="s" s="6">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s" s="6">
+      <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" t="s" s="6">
+      <c r="F6" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" t="s" s="6">
+      <c r="H6" s="6" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="5">
         <v>3</v>
       </c>
       <c r="B7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" t="s" s="6">
+      <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s" s="6">
+      <c r="D7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s" s="6">
+      <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F7" t="s" s="6">
+      <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" t="s" s="6">
+      <c r="G7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H7" t="s" s="6">
+      <c r="H7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I7" t="s" s="6">
+      <c r="I7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:9" ht="17" customHeight="1">
       <c r="A8" s="5">
         <v>4</v>
       </c>
       <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" t="s" s="6">
+      <c r="C8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s" s="6">
+      <c r="D8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s" s="6">
+      <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F8" t="s" s="6">
+      <c r="F8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G8" t="s" s="6">
+      <c r="G8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H8" t="s" s="6">
+      <c r="H8" s="6" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:9" ht="17" customHeight="1">
       <c r="A9" s="5">
         <v>4</v>
       </c>
       <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" t="s" s="6">
+      <c r="C9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s" s="6">
+      <c r="D9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s" s="6">
+      <c r="E9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" t="s" s="6">
+      <c r="G9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H9" t="s" s="6">
+      <c r="H9" s="6" t="s">
         <v>27</v>
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:9" ht="17" customHeight="1">
       <c r="A10" s="5">
         <v>5</v>
       </c>
       <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" t="s" s="6">
+      <c r="C10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D10" t="s" s="6">
+      <c r="D10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s" s="6">
+      <c r="E10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F10" t="s" s="6">
+      <c r="F10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G10" t="s" s="6">
+      <c r="G10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H10" t="s" s="7">
+      <c r="H10" s="7" t="s">
         <v>43</v>
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" ht="17" customHeight="1">
+    <row r="11" spans="1:9" ht="17" customHeight="1">
       <c r="A11" s="5">
         <v>5</v>
       </c>
       <c r="B11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" t="s" s="6">
+      <c r="C11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s" s="8">
+      <c r="D11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E11" t="s" s="8">
+      <c r="E11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" t="s" s="6">
+      <c r="G11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" ht="17" customHeight="1">
-      <c r="A12" t="s" s="3">
+    <row r="12" spans="1:9" ht="17" customHeight="1">
+      <c r="A12" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="5"/>
@@ -1970,226 +2018,224 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" ht="17" customHeight="1">
+    <row r="13" spans="1:9" ht="17" customHeight="1">
       <c r="A13" s="5">
         <v>6</v>
       </c>
       <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" t="s" s="6">
+      <c r="C13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D13" t="s" s="6">
+      <c r="D13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E13" t="s" s="6">
+      <c r="E13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F13" t="s" s="6">
+      <c r="F13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G13" t="s" s="6">
+      <c r="G13" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" ht="17" customHeight="1">
+    <row r="14" spans="1:9" ht="17" customHeight="1">
       <c r="A14" s="5">
         <v>6</v>
       </c>
       <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" t="s" s="6">
+      <c r="C14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D14" t="s" s="6">
+      <c r="D14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E14" t="s" s="6">
+      <c r="E14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" t="s" s="6">
+      <c r="G14" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" ht="17" customHeight="1">
+    <row r="15" spans="1:9" ht="17" customHeight="1">
       <c r="A15" s="5">
         <v>7</v>
       </c>
       <c r="B15" s="5">
         <v>11</v>
       </c>
-      <c r="C15" t="s" s="6">
+      <c r="C15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D15" t="s" s="6">
-        <v>53</v>
-      </c>
-      <c r="E15" t="s" s="6">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s" s="6">
-        <v>54</v>
-      </c>
-      <c r="G15" t="s" s="6">
+      <c r="D15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" ht="17" customHeight="1">
+    <row r="16" spans="1:9" ht="17" customHeight="1">
       <c r="A16" s="5">
         <v>7</v>
       </c>
       <c r="B16" s="5">
         <v>12</v>
       </c>
-      <c r="C16" t="s" s="6">
+      <c r="C16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D16" t="s" s="6">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s" s="6">
+      <c r="E16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="5"/>
-      <c r="G16" t="s" s="6">
+      <c r="G16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" ht="17" customHeight="1">
+    <row r="17" spans="1:9" ht="17" customHeight="1">
       <c r="A17" s="5">
         <v>8</v>
       </c>
       <c r="B17" s="5">
         <v>13</v>
       </c>
-      <c r="C17" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="D17" t="s" s="6">
-        <v>58</v>
-      </c>
-      <c r="E17" t="s" s="6">
-        <v>59</v>
-      </c>
-      <c r="F17" t="s" s="6">
-        <v>60</v>
-      </c>
-      <c r="G17" t="s" s="6">
+      <c r="C17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" ht="17" customHeight="1">
+    </row>
+    <row r="18" spans="1:9" ht="17" customHeight="1">
       <c r="A18" s="5">
         <v>8</v>
       </c>
       <c r="B18" s="5">
         <v>14</v>
       </c>
-      <c r="C18" t="s" s="6">
-        <v>61</v>
-      </c>
-      <c r="D18" t="s" s="8">
-        <v>62</v>
-      </c>
-      <c r="E18" t="s" s="8">
+      <c r="C18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F18" s="5"/>
-      <c r="G18" t="s" s="6">
+      <c r="G18" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" ht="17" customHeight="1">
+    <row r="19" spans="1:9" ht="17" customHeight="1">
       <c r="A19" s="5">
         <v>9</v>
       </c>
       <c r="B19" s="5">
         <v>15</v>
       </c>
-      <c r="C19" t="s" s="6">
-        <v>63</v>
-      </c>
-      <c r="D19" t="s" s="6">
+      <c r="C19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E19" t="s" s="6">
-        <v>30</v>
-      </c>
-      <c r="F19" t="s" s="6">
-        <v>64</v>
-      </c>
-      <c r="G19" t="s" s="6">
+      <c r="G19" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" ht="17" customHeight="1">
+    <row r="20" spans="1:9" ht="17" customHeight="1">
       <c r="A20" s="5">
         <v>9</v>
       </c>
       <c r="B20" s="5">
         <v>16</v>
       </c>
-      <c r="C20" t="s" s="6">
-        <v>65</v>
-      </c>
-      <c r="D20" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="E20" t="s" s="6">
+      <c r="C20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="5"/>
-      <c r="G20" t="s" s="6">
+      <c r="G20" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" ht="17" customHeight="1">
+    <row r="21" spans="1:9" ht="17" customHeight="1">
       <c r="A21" s="5">
         <v>10</v>
       </c>
       <c r="B21" s="5">
         <v>17</v>
       </c>
-      <c r="C21" t="s" s="6">
+      <c r="C21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D21" t="s" s="6">
-        <v>68</v>
-      </c>
-      <c r="E21" t="s" s="6">
-        <v>12</v>
-      </c>
-      <c r="F21" t="s" s="6">
-        <v>69</v>
-      </c>
-      <c r="G21" t="s" s="6">
+      <c r="G21" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" ht="17" customHeight="1">
-      <c r="A22" t="s" s="3">
-        <v>70</v>
+    <row r="22" spans="1:9" ht="17" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2200,223 +2246,223 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" ht="17" customHeight="1">
+    <row r="23" spans="1:9" ht="17" customHeight="1">
       <c r="A23" s="5">
         <v>10</v>
       </c>
       <c r="B23" s="5">
         <v>18</v>
       </c>
-      <c r="C23" t="s" s="6">
-        <v>71</v>
-      </c>
-      <c r="D23" t="s" s="6">
-        <v>72</v>
-      </c>
-      <c r="E23" t="s" s="6">
+      <c r="C23" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="5"/>
-      <c r="G23" t="s" s="6">
+      <c r="G23" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" ht="17" customHeight="1">
+    <row r="24" spans="1:9" ht="17" customHeight="1">
       <c r="A24" s="5">
         <v>11</v>
       </c>
       <c r="B24" s="5">
         <v>19</v>
       </c>
-      <c r="C24" t="s" s="6">
+      <c r="C24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D24" t="s" s="6">
-        <v>74</v>
-      </c>
-      <c r="E24" t="s" s="6">
-        <v>12</v>
-      </c>
-      <c r="F24" t="s" s="6">
-        <v>75</v>
-      </c>
-      <c r="G24" t="s" s="6">
+      <c r="G24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" ht="17" customHeight="1">
+    <row r="25" spans="1:9" ht="17" customHeight="1">
       <c r="A25" s="5">
         <v>11</v>
       </c>
       <c r="B25" s="5">
         <v>20</v>
       </c>
-      <c r="C25" t="s" s="6">
+      <c r="C25" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D25" t="s" s="8">
-        <v>77</v>
-      </c>
-      <c r="E25" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="G25" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="H25" t="s" s="6">
-        <v>78</v>
-      </c>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" ht="17" customHeight="1">
+    <row r="26" spans="1:9" ht="17" customHeight="1">
       <c r="A26" s="5">
         <v>12</v>
       </c>
       <c r="B26" s="5">
         <v>21</v>
       </c>
-      <c r="C26" t="s" s="6">
+      <c r="C26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D26" t="s" s="8">
-        <v>80</v>
-      </c>
-      <c r="E26" t="s" s="8">
-        <v>81</v>
-      </c>
       <c r="F26" s="5"/>
-      <c r="G26" t="s" s="6">
+      <c r="G26" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" ht="17" customHeight="1">
+    <row r="27" spans="1:9" ht="17" customHeight="1">
       <c r="A27" s="5">
         <v>12</v>
       </c>
       <c r="B27" s="5">
         <v>22</v>
       </c>
-      <c r="C27" t="s" s="6">
+      <c r="C27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D27" t="s" s="6">
-        <v>83</v>
-      </c>
-      <c r="E27" t="s" s="6">
-        <v>84</v>
-      </c>
       <c r="F27" s="5"/>
-      <c r="G27" t="s" s="6">
+      <c r="G27" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" ht="17" customHeight="1">
+    <row r="28" spans="1:9" ht="17" customHeight="1">
       <c r="A28" s="5">
         <v>13</v>
       </c>
       <c r="B28" s="5">
         <v>23</v>
       </c>
-      <c r="C28" t="s" s="6">
+      <c r="C28" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D28" t="s" s="8">
-        <v>86</v>
-      </c>
-      <c r="E28" t="s" s="8">
-        <v>87</v>
-      </c>
       <c r="F28" s="5"/>
-      <c r="G28" t="s" s="6">
+      <c r="G28" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" ht="17" customHeight="1">
+    <row r="29" spans="1:9" ht="17" customHeight="1">
       <c r="A29" s="5">
         <v>13</v>
       </c>
       <c r="B29" s="5">
         <v>24</v>
       </c>
-      <c r="C29" t="s" s="6">
-        <v>88</v>
-      </c>
-      <c r="D29" t="s" s="6">
-        <v>89</v>
-      </c>
-      <c r="E29" t="s" s="6">
+      <c r="C29" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="5"/>
-      <c r="G29" t="s" s="6">
+      <c r="G29" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" ht="17" customHeight="1">
+    <row r="30" spans="1:9" ht="17" customHeight="1">
       <c r="A30" s="5">
         <v>14</v>
       </c>
       <c r="B30" s="5">
         <v>25</v>
       </c>
-      <c r="C30" t="s" s="6">
-        <v>90</v>
-      </c>
-      <c r="D30" t="s" s="6">
-        <v>91</v>
-      </c>
-      <c r="E30" t="s" s="6">
+      <c r="C30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="5"/>
-      <c r="G30" t="s" s="6">
+      <c r="G30" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" ht="17" customHeight="1">
+    <row r="31" spans="1:9" ht="17" customHeight="1">
       <c r="A31" s="5">
         <v>14</v>
       </c>
       <c r="B31" s="5"/>
-      <c r="C31" t="s" s="6">
-        <v>92</v>
-      </c>
-      <c r="D31" t="s" s="6">
+      <c r="C31" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" t="s" s="6">
-        <v>93</v>
+      <c r="F31" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" ht="17" customHeight="1">
+    <row r="32" spans="1:9" ht="17" customHeight="1">
       <c r="A32" s="5">
         <v>15</v>
       </c>
       <c r="B32" s="5"/>
-      <c r="C32" t="s" s="6">
-        <v>94</v>
-      </c>
-      <c r="D32" t="s" s="6">
-        <v>95</v>
+      <c r="C32" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -2424,16 +2470,16 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" ht="17" customHeight="1">
+    <row r="33" spans="1:9" ht="17" customHeight="1">
       <c r="A33" s="5">
         <v>15</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" t="s" s="6">
-        <v>96</v>
-      </c>
-      <c r="D33" t="s" s="6">
-        <v>95</v>
+      <c r="C33" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -2441,45 +2487,45 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" ht="17" customHeight="1">
+    <row r="34" spans="1:9" ht="17" customHeight="1">
       <c r="A34" s="5">
         <v>16</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" t="s" s="6">
+      <c r="C34" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="D34" t="s" s="6">
-        <v>98</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" t="s" s="6">
-        <v>99</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" ht="17" customHeight="1">
+    <row r="35" spans="1:9" ht="17" customHeight="1">
       <c r="A35" s="5">
         <v>16</v>
       </c>
       <c r="B35" s="5"/>
-      <c r="C35" t="s" s="6">
-        <v>100</v>
-      </c>
-      <c r="D35" t="s" s="6">
+      <c r="C35" s="6" t="s">
         <v>98</v>
       </c>
+      <c r="D35" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="E35" s="5"/>
-      <c r="F35" t="s" s="6">
-        <v>99</v>
+      <c r="F35" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" ht="17" customHeight="1">
+    <row r="36" spans="1:9" ht="17" customHeight="1">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2490,7 +2536,7 @@
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" ht="17" customHeight="1">
+    <row r="37" spans="1:9" ht="17" customHeight="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2501,7 +2547,7 @@
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" ht="17" customHeight="1">
+    <row r="38" spans="1:9" ht="17" customHeight="1">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2512,7 +2558,7 @@
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" ht="17" customHeight="1">
+    <row r="39" spans="1:9" ht="17" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2523,7 +2569,7 @@
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" ht="17" customHeight="1">
+    <row r="40" spans="1:9" ht="17" customHeight="1">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2534,9 +2580,9 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" ht="17" customHeight="1">
-      <c r="A41" t="s" s="10">
-        <v>101</v>
+    <row r="41" spans="1:9" ht="17" customHeight="1">
+      <c r="A41" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="4"/>
@@ -2547,529 +2593,529 @@
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" ht="30" customHeight="1">
+    <row r="42" spans="1:9" ht="30" customHeight="1">
       <c r="A42" s="5">
         <v>1</v>
       </c>
       <c r="B42" s="5"/>
-      <c r="C42" t="s" s="6">
+      <c r="C42" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D42" t="s" s="6">
-        <v>102</v>
+      <c r="D42" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="E42" s="5"/>
-      <c r="F42" t="s" s="6">
-        <v>103</v>
+      <c r="F42" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" ht="17" customHeight="1">
+    <row r="43" spans="1:9" ht="17" customHeight="1">
       <c r="A43" s="5">
         <v>2</v>
       </c>
       <c r="B43" s="5"/>
-      <c r="C43" t="s" s="6">
+      <c r="C43" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D43" t="s" s="6">
+      <c r="D43" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E43" s="5"/>
-      <c r="F43" t="s" s="6">
-        <v>104</v>
+      <c r="F43" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" ht="17" customHeight="1">
+    <row r="44" spans="1:9" ht="17" customHeight="1">
       <c r="A44" s="5">
         <v>2</v>
       </c>
       <c r="B44" s="5"/>
-      <c r="C44" t="s" s="6">
+      <c r="C44" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D44" t="s" s="6">
-        <v>105</v>
+      <c r="D44" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="E44" s="5"/>
-      <c r="F44" t="s" s="6">
-        <v>106</v>
+      <c r="F44" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" ht="17" customHeight="1">
+    <row r="45" spans="1:9" ht="17" customHeight="1">
       <c r="A45" s="5">
         <v>3</v>
       </c>
       <c r="B45" s="5"/>
-      <c r="C45" t="s" s="6">
+      <c r="C45" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D45" t="s" s="6">
+      <c r="D45" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E45" s="5"/>
-      <c r="F45" t="s" s="6">
+      <c r="F45" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" ht="17" customHeight="1">
+    <row r="46" spans="1:9" ht="17" customHeight="1">
       <c r="A46" s="5">
         <v>3</v>
       </c>
       <c r="B46" s="5"/>
-      <c r="C46" t="s" s="6">
+      <c r="C46" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D46" t="s" s="6">
+      <c r="D46" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E46" s="5"/>
-      <c r="F46" t="s" s="6">
-        <v>107</v>
+      <c r="F46" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" ht="17" customHeight="1">
+    <row r="47" spans="1:9" ht="17" customHeight="1">
       <c r="A47" s="5">
         <v>4</v>
       </c>
       <c r="B47" s="5"/>
-      <c r="C47" t="s" s="6">
+      <c r="C47" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D47" t="s" s="6">
-        <v>108</v>
+      <c r="D47" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="E47" s="5"/>
-      <c r="F47" t="s" s="6">
-        <v>109</v>
+      <c r="F47" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" ht="17" customHeight="1">
+    <row r="48" spans="1:9" ht="17" customHeight="1">
       <c r="A48" s="5">
         <v>4</v>
       </c>
       <c r="B48" s="5"/>
-      <c r="C48" t="s" s="6">
+      <c r="C48" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D48" t="s" s="6">
-        <v>110</v>
+      <c r="D48" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="E48" s="5"/>
-      <c r="F48" t="s" s="6">
-        <v>104</v>
+      <c r="F48" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" ht="17" customHeight="1">
+    <row r="49" spans="1:9" ht="17" customHeight="1">
       <c r="A49" s="5">
         <v>5</v>
       </c>
       <c r="B49" s="5"/>
-      <c r="C49" t="s" s="6">
+      <c r="C49" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D49" t="s" s="6">
-        <v>108</v>
+      <c r="D49" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="E49" s="5"/>
-      <c r="F49" t="s" s="6">
-        <v>111</v>
+      <c r="F49" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
-    <row r="50" ht="17" customHeight="1">
+    <row r="50" spans="1:9" ht="17" customHeight="1">
       <c r="A50" s="5">
         <v>5</v>
       </c>
       <c r="B50" s="5"/>
-      <c r="C50" t="s" s="6">
+      <c r="C50" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D50" t="s" s="8">
-        <v>112</v>
+      <c r="D50" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="E50" s="12"/>
-      <c r="F50" t="s" s="6">
-        <v>104</v>
+      <c r="F50" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
     </row>
-    <row r="51" ht="17" customHeight="1">
+    <row r="51" spans="1:9" ht="17" customHeight="1">
       <c r="A51" s="5">
         <v>6</v>
       </c>
       <c r="B51" s="5"/>
-      <c r="C51" t="s" s="6">
+      <c r="C51" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D51" t="s" s="6">
-        <v>113</v>
+      <c r="D51" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="E51" s="5"/>
-      <c r="F51" t="s" s="6">
-        <v>104</v>
+      <c r="F51" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" ht="17" customHeight="1">
+    <row r="52" spans="1:9" ht="17" customHeight="1">
       <c r="A52" s="5">
         <v>6</v>
       </c>
       <c r="B52" s="5"/>
-      <c r="C52" t="s" s="6">
+      <c r="C52" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D52" t="s" s="6">
-        <v>114</v>
+      <c r="D52" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="E52" s="5"/>
-      <c r="F52" t="s" s="6">
-        <v>115</v>
+      <c r="F52" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
     </row>
-    <row r="53" ht="17" customHeight="1">
+    <row r="53" spans="1:9" ht="17" customHeight="1">
       <c r="A53" s="5">
         <v>7</v>
       </c>
       <c r="B53" s="5"/>
-      <c r="C53" t="s" s="6">
+      <c r="C53" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D53" t="s" s="6">
-        <v>113</v>
+      <c r="D53" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="E53" s="5"/>
-      <c r="F53" t="s" s="6">
-        <v>116</v>
+      <c r="F53" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
     </row>
-    <row r="54" ht="17" customHeight="1">
+    <row r="54" spans="1:9" ht="17" customHeight="1">
       <c r="A54" s="5">
         <v>7</v>
       </c>
       <c r="B54" s="5"/>
-      <c r="C54" t="s" s="6">
-        <v>55</v>
-      </c>
-      <c r="D54" t="s" s="6">
-        <v>117</v>
+      <c r="C54" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="E54" s="5"/>
-      <c r="F54" t="s" s="6">
-        <v>118</v>
+      <c r="F54" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
     </row>
-    <row r="55" ht="17" customHeight="1">
+    <row r="55" spans="1:9" ht="17" customHeight="1">
       <c r="A55" s="5">
         <v>8</v>
       </c>
       <c r="B55" s="5"/>
-      <c r="C55" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="D55" t="s" s="6">
-        <v>119</v>
+      <c r="C55" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="E55" s="5"/>
-      <c r="F55" t="s" s="6">
-        <v>104</v>
+      <c r="F55" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
     </row>
-    <row r="56" ht="17" customHeight="1">
+    <row r="56" spans="1:9" ht="17" customHeight="1">
       <c r="A56" s="5">
         <v>8</v>
       </c>
       <c r="B56" s="5"/>
-      <c r="C56" t="s" s="6">
-        <v>61</v>
-      </c>
-      <c r="D56" t="s" s="6">
-        <v>120</v>
+      <c r="C56" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="E56" s="5"/>
-      <c r="F56" t="s" s="6">
-        <v>104</v>
+      <c r="F56" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
     </row>
-    <row r="57" ht="17" customHeight="1">
+    <row r="57" spans="1:9" ht="17" customHeight="1">
       <c r="A57" s="5">
         <v>9</v>
       </c>
       <c r="B57" s="5"/>
-      <c r="C57" t="s" s="6">
-        <v>63</v>
-      </c>
-      <c r="D57" t="s" s="6">
-        <v>121</v>
+      <c r="C57" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="E57" s="5"/>
-      <c r="F57" t="s" s="6">
-        <v>122</v>
+      <c r="F57" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
     </row>
-    <row r="58" ht="30" customHeight="1">
+    <row r="58" spans="1:9" ht="30" customHeight="1">
       <c r="A58" s="5">
         <v>9</v>
       </c>
       <c r="B58" s="5"/>
-      <c r="C58" t="s" s="6">
-        <v>65</v>
-      </c>
-      <c r="D58" t="s" s="6">
-        <v>123</v>
+      <c r="C58" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="E58" s="5"/>
-      <c r="F58" t="s" s="6">
-        <v>124</v>
+      <c r="F58" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
     </row>
-    <row r="59" ht="17" customHeight="1">
+    <row r="59" spans="1:9" ht="17" customHeight="1">
       <c r="A59" s="5">
         <v>10</v>
       </c>
       <c r="B59" s="5"/>
-      <c r="C59" t="s" s="6">
-        <v>67</v>
-      </c>
-      <c r="D59" t="s" s="6">
-        <v>125</v>
+      <c r="C59" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="E59" s="5"/>
-      <c r="F59" t="s" s="6">
-        <v>106</v>
+      <c r="F59" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" ht="17" customHeight="1">
+    <row r="60" spans="1:9" ht="17" customHeight="1">
       <c r="A60" s="5">
         <v>10</v>
       </c>
       <c r="B60" s="5"/>
-      <c r="C60" t="s" s="6">
-        <v>71</v>
-      </c>
-      <c r="D60" t="s" s="6">
-        <v>125</v>
+      <c r="C60" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="E60" s="5"/>
-      <c r="F60" t="s" s="6">
-        <v>126</v>
+      <c r="F60" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" ht="17" customHeight="1">
+    <row r="61" spans="1:9" ht="17" customHeight="1">
       <c r="A61" s="5">
         <v>11</v>
       </c>
       <c r="B61" s="5"/>
-      <c r="C61" t="s" s="6">
-        <v>73</v>
-      </c>
-      <c r="D61" t="s" s="6">
-        <v>127</v>
+      <c r="C61" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="E61" s="5"/>
-      <c r="F61" t="s" s="6">
-        <v>106</v>
+      <c r="F61" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
     </row>
-    <row r="62" ht="17" customHeight="1">
+    <row r="62" spans="1:9" ht="17" customHeight="1">
       <c r="A62" s="5">
         <v>11</v>
       </c>
       <c r="B62" s="5"/>
-      <c r="C62" t="s" s="6">
-        <v>76</v>
-      </c>
-      <c r="D62" t="s" s="6">
-        <v>128</v>
+      <c r="C62" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="E62" s="5"/>
-      <c r="F62" t="s" s="6">
-        <v>129</v>
+      <c r="F62" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
     </row>
-    <row r="63" ht="17" customHeight="1">
+    <row r="63" spans="1:9" ht="17" customHeight="1">
       <c r="A63" s="5">
         <v>12</v>
       </c>
       <c r="B63" s="5"/>
-      <c r="C63" t="s" s="6">
-        <v>79</v>
-      </c>
-      <c r="D63" t="s" s="6">
-        <v>130</v>
+      <c r="C63" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="E63" s="5"/>
-      <c r="F63" t="s" s="6">
-        <v>106</v>
+      <c r="F63" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
     </row>
-    <row r="64" ht="17" customHeight="1">
+    <row r="64" spans="1:9" ht="17" customHeight="1">
       <c r="A64" s="5">
         <v>12</v>
       </c>
       <c r="B64" s="5"/>
-      <c r="C64" t="s" s="6">
-        <v>82</v>
-      </c>
-      <c r="D64" t="s" s="6">
+      <c r="C64" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E64" s="5"/>
-      <c r="F64" t="s" s="6">
-        <v>131</v>
+      <c r="F64" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" ht="17" customHeight="1">
+    <row r="65" spans="1:9" ht="17" customHeight="1">
       <c r="A65" s="5">
         <v>13</v>
       </c>
       <c r="B65" s="5"/>
-      <c r="C65" t="s" s="6">
-        <v>85</v>
-      </c>
-      <c r="D65" t="s" s="6">
-        <v>132</v>
+      <c r="C65" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="E65" s="5"/>
-      <c r="F65" t="s" s="6">
-        <v>133</v>
+      <c r="F65" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
     </row>
-    <row r="66" ht="17" customHeight="1">
+    <row r="66" spans="1:9" ht="17" customHeight="1">
       <c r="A66" s="5">
         <v>13</v>
       </c>
       <c r="B66" s="5"/>
-      <c r="C66" t="s" s="6">
-        <v>88</v>
-      </c>
-      <c r="D66" t="s" s="6">
-        <v>134</v>
+      <c r="C66" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="E66" s="5"/>
-      <c r="F66" t="s" s="6">
-        <v>104</v>
+      <c r="F66" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
     </row>
-    <row r="67" ht="17" customHeight="1">
+    <row r="67" spans="1:9" ht="17" customHeight="1">
       <c r="A67" s="5">
         <v>14</v>
       </c>
       <c r="B67" s="5"/>
-      <c r="C67" t="s" s="6">
-        <v>90</v>
-      </c>
-      <c r="D67" t="s" s="6">
-        <v>135</v>
+      <c r="C67" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="E67" s="5"/>
-      <c r="F67" t="s" s="6">
-        <v>104</v>
+      <c r="F67" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" ht="17" customHeight="1">
+    <row r="68" spans="1:9" ht="17" customHeight="1">
       <c r="A68" s="5">
         <v>14</v>
       </c>
       <c r="B68" s="5"/>
-      <c r="C68" t="s" s="6">
-        <v>92</v>
-      </c>
-      <c r="D68" t="s" s="6">
+      <c r="C68" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E68" s="5"/>
-      <c r="F68" t="s" s="6">
-        <v>93</v>
+      <c r="F68" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
-    <row r="69" ht="17" customHeight="1">
+    <row r="69" spans="1:9" ht="17" customHeight="1">
       <c r="A69" s="5">
         <v>15</v>
       </c>
       <c r="B69" s="5"/>
-      <c r="C69" t="s" s="6">
-        <v>94</v>
-      </c>
-      <c r="D69" t="s" s="6">
-        <v>95</v>
+      <c r="C69" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
@@ -3077,16 +3123,16 @@
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
     </row>
-    <row r="70" ht="17" customHeight="1">
+    <row r="70" spans="1:9" ht="17" customHeight="1">
       <c r="A70" s="5">
         <v>15</v>
       </c>
       <c r="B70" s="5"/>
-      <c r="C70" t="s" s="6">
-        <v>96</v>
-      </c>
-      <c r="D70" t="s" s="6">
-        <v>95</v>
+      <c r="C70" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -3094,73 +3140,73 @@
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
-    <row r="71" ht="17" customHeight="1">
+    <row r="71" spans="1:9" ht="17" customHeight="1">
       <c r="A71" s="5">
         <v>16</v>
       </c>
       <c r="B71" s="5"/>
-      <c r="C71" t="s" s="6">
+      <c r="C71" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E71" s="5"/>
+      <c r="F71" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="D71" t="s" s="6">
-        <v>98</v>
-      </c>
-      <c r="E71" s="5"/>
-      <c r="F71" t="s" s="6">
-        <v>99</v>
       </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
-    <row r="72" ht="17" customHeight="1">
+    <row r="72" spans="1:9" ht="17" customHeight="1">
       <c r="A72" s="5">
         <v>16</v>
       </c>
       <c r="B72" s="5"/>
-      <c r="C72" t="s" s="6">
-        <v>100</v>
-      </c>
-      <c r="D72" t="s" s="6">
+      <c r="C72" s="6" t="s">
         <v>98</v>
       </c>
+      <c r="D72" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="E72" s="5"/>
-      <c r="F72" t="s" s="6">
-        <v>99</v>
+      <c r="F72" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" ht="17" customHeight="1">
+    <row r="73" spans="1:9" ht="17" customHeight="1">
       <c r="A73" s="5">
         <v>17</v>
       </c>
       <c r="B73" s="5"/>
-      <c r="C73" t="s" s="6">
-        <v>136</v>
+      <c r="C73" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
-      <c r="F73" t="s" s="6">
-        <v>137</v>
+      <c r="F73" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" ht="17" customHeight="1">
+    <row r="74" spans="1:9" ht="17" customHeight="1">
       <c r="A74" s="5">
         <v>18</v>
       </c>
       <c r="B74" s="5"/>
-      <c r="C74" t="s" s="6">
-        <v>138</v>
+      <c r="C74" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
-      <c r="F74" t="s" s="6">
-        <v>137</v>
+      <c r="F74" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
@@ -3168,9 +3214,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>